<commit_message>
correciones del campo sexo
</commit_message>
<xml_diff>
--- a/comisiones_alc/afiliaciones/excel/Personal ACE.xlsx
+++ b/comisiones_alc/afiliaciones/excel/Personal ACE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\Desktop\ACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D421A7B-49D6-4FD7-902B-193CD7AABBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EFA860-2F55-4727-8382-8200D6F0280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FA675B1F-6BC5-44B1-A200-E8E4A6E8D909}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="284">
   <si>
     <t>DIRECTOR GENERAL</t>
   </si>
@@ -880,6 +880,15 @@
   </si>
   <si>
     <t>CORREO</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -889,7 +898,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,6 +992,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1016,7 +1039,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1065,13 +1088,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1167,10 +1199,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1947,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58124BF6-347E-4826-A0B0-718778408EB1}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1959,32 +1997,36 @@
     <col min="2" max="2" width="47.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="24.88671875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="66.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="62.88671875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.44140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="65.21875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" customWidth="1"/>
+    <col min="8" max="8" width="11" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="36"/>
-    </row>
-    <row r="12" spans="1:7" s="10" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-    </row>
-    <row r="13" spans="1:7" s="9" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+    </row>
+    <row r="13" spans="1:8" s="9" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>131</v>
       </c>
@@ -2006,8 +2048,11 @@
       <c r="G13" s="23" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="39" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>1</v>
       </c>
@@ -2029,8 +2074,11 @@
       <c r="G14" s="15" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>2</v>
       </c>
@@ -2052,8 +2100,11 @@
       <c r="G15" s="15" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>3</v>
       </c>
@@ -2075,8 +2126,11 @@
       <c r="G16" s="15" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>4</v>
       </c>
@@ -2098,8 +2152,11 @@
       <c r="G17" s="15" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>5</v>
       </c>
@@ -2121,8 +2178,11 @@
       <c r="G18" s="15" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>6</v>
       </c>
@@ -2144,8 +2204,11 @@
       <c r="G19" s="15" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>7</v>
       </c>
@@ -2167,8 +2230,11 @@
       <c r="G20" s="15" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>8</v>
       </c>
@@ -2190,8 +2256,11 @@
       <c r="G21" s="15" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>9</v>
       </c>
@@ -2213,8 +2282,11 @@
       <c r="G22" s="15" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H22" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>10</v>
       </c>
@@ -2236,8 +2308,11 @@
       <c r="G23" s="15" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>11</v>
       </c>
@@ -2259,8 +2334,11 @@
       <c r="G24" s="15" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>12</v>
       </c>
@@ -2282,8 +2360,11 @@
       <c r="G25" s="15" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>13</v>
       </c>
@@ -2305,8 +2386,11 @@
       <c r="G26" s="15" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>14</v>
       </c>
@@ -2328,8 +2412,11 @@
       <c r="G27" s="15" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>15</v>
       </c>
@@ -2351,8 +2438,11 @@
       <c r="G28" s="15" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>16</v>
       </c>
@@ -2374,8 +2464,11 @@
       <c r="G29" s="15" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>17</v>
       </c>
@@ -2397,8 +2490,11 @@
       <c r="G30" s="15" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>18</v>
       </c>
@@ -2420,8 +2516,11 @@
       <c r="G31" s="15" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H31" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>19</v>
       </c>
@@ -2443,8 +2542,11 @@
       <c r="G32" s="15" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>20</v>
       </c>
@@ -2466,8 +2568,11 @@
       <c r="G33" s="15" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H33" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>21</v>
       </c>
@@ -2489,8 +2594,11 @@
       <c r="G34" s="15" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H34" s="41" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
         <v>22</v>
       </c>
@@ -2512,8 +2620,11 @@
       <c r="G35" s="15" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H35" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>23</v>
       </c>
@@ -2535,8 +2646,11 @@
       <c r="G36" s="15" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H36" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
         <v>24</v>
       </c>
@@ -2558,8 +2672,11 @@
       <c r="G37" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H37" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>25</v>
       </c>
@@ -2581,8 +2698,11 @@
       <c r="G38" s="15" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>26</v>
       </c>
@@ -2604,8 +2724,11 @@
       <c r="G39" s="15" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H39" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>27</v>
       </c>
@@ -2627,8 +2750,11 @@
       <c r="G40" s="15" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H40" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11">
         <v>28</v>
       </c>
@@ -2650,8 +2776,11 @@
       <c r="G41" s="15" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H41" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>29</v>
       </c>
@@ -2673,8 +2802,11 @@
       <c r="G42" s="15" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H42" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
         <v>30</v>
       </c>
@@ -2696,8 +2828,11 @@
       <c r="G43" s="15" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H43" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>31</v>
       </c>
@@ -2719,8 +2854,11 @@
       <c r="G44" s="15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H44" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>32</v>
       </c>
@@ -2742,8 +2880,11 @@
       <c r="G45" s="15" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H45" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>33</v>
       </c>
@@ -2765,8 +2906,11 @@
       <c r="G46" s="15" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H46" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
         <v>34</v>
       </c>
@@ -2788,8 +2932,11 @@
       <c r="G47" s="15" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H47" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>35</v>
       </c>
@@ -2811,8 +2958,11 @@
       <c r="G48" s="15" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H48" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>36</v>
       </c>
@@ -2834,8 +2984,11 @@
       <c r="G49" s="15" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H49" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>37</v>
       </c>
@@ -2857,8 +3010,11 @@
       <c r="G50" s="15" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H50" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>38</v>
       </c>
@@ -2880,8 +3036,11 @@
       <c r="G51" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H51" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>39</v>
       </c>
@@ -2903,8 +3062,11 @@
       <c r="G52" s="15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H52" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>40</v>
       </c>
@@ -2926,8 +3088,11 @@
       <c r="G53" s="15" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H53" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>41</v>
       </c>
@@ -2949,8 +3114,11 @@
       <c r="G54" s="15" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H54" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>42</v>
       </c>
@@ -2972,8 +3140,11 @@
       <c r="G55" s="15" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H55" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>43</v>
       </c>
@@ -2995,8 +3166,11 @@
       <c r="G56" s="15" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H56" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>44</v>
       </c>
@@ -3018,8 +3192,11 @@
       <c r="G57" s="15" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H57" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
         <v>45</v>
       </c>
@@ -3041,8 +3218,11 @@
       <c r="G58" s="15" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H58" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="11">
         <v>46</v>
       </c>
@@ -3064,8 +3244,11 @@
       <c r="G59" s="15" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H59" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="11">
         <v>47</v>
       </c>
@@ -3087,8 +3270,11 @@
       <c r="G60" s="15" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H60" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="11">
         <v>48</v>
       </c>
@@ -3110,8 +3296,11 @@
       <c r="G61" s="15" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H61" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>49</v>
       </c>
@@ -3133,8 +3322,11 @@
       <c r="G62" s="15" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H62" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
         <v>50</v>
       </c>
@@ -3156,8 +3348,11 @@
       <c r="G63" s="15" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H63" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
         <v>51</v>
       </c>
@@ -3179,8 +3374,11 @@
       <c r="G64" s="15" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H64" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="11">
         <v>52</v>
       </c>
@@ -3202,8 +3400,11 @@
       <c r="G65" s="15" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H65" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11">
         <v>53</v>
       </c>
@@ -3225,8 +3426,11 @@
       <c r="G66" s="15" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H66" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="11">
         <v>54</v>
       </c>
@@ -3245,11 +3449,14 @@
       <c r="F67" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G67" s="38" t="s">
+      <c r="G67" s="37" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H67" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="11">
         <v>55</v>
       </c>
@@ -3268,11 +3475,14 @@
       <c r="F68" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G68" s="38" t="s">
+      <c r="G68" s="37" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H68" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11">
         <v>56</v>
       </c>
@@ -3291,11 +3501,14 @@
       <c r="F69" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G69" s="38" t="s">
+      <c r="G69" s="37" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H69" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="11">
         <v>57</v>
       </c>
@@ -3314,11 +3527,14 @@
       <c r="F70" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G70" s="38" t="s">
+      <c r="G70" s="37" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="11">
         <v>58</v>
       </c>
@@ -3340,8 +3556,11 @@
       <c r="G71" s="15" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H71" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="11">
         <v>59</v>
       </c>
@@ -3363,8 +3582,11 @@
       <c r="G72" s="15" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H72" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="11">
         <v>60</v>
       </c>
@@ -3386,8 +3608,11 @@
       <c r="G73" s="15" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H73" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="11">
         <v>61</v>
       </c>
@@ -3409,8 +3634,11 @@
       <c r="G74" s="15" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H74" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11">
         <v>62</v>
       </c>
@@ -3432,8 +3660,11 @@
       <c r="G75" s="15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H75" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11">
         <v>63</v>
       </c>
@@ -3455,8 +3686,11 @@
       <c r="G76" s="15" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H76" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="11">
         <v>64</v>
       </c>
@@ -3478,8 +3712,11 @@
       <c r="G77" s="15" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H77" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11">
         <v>65</v>
       </c>
@@ -3498,11 +3735,14 @@
       <c r="F78" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G78" s="38" t="s">
+      <c r="G78" s="37" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H78" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="11">
         <v>66</v>
       </c>
@@ -3524,8 +3764,11 @@
       <c r="G79" s="15" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H79" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11">
         <v>67</v>
       </c>
@@ -3547,42 +3790,49 @@
       <c r="G80" s="15" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H80" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
-    </row>
-    <row r="82" spans="1:6" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H81" s="38"/>
+    </row>
+    <row r="82" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
-    </row>
-    <row r="83" spans="1:6" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H82" s="38"/>
+    </row>
+    <row r="83" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
-    </row>
-    <row r="84" spans="1:6" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H83" s="38"/>
+    </row>
+    <row r="84" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
+      <c r="H84" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <conditionalFormatting sqref="B14 B20:B21">
     <cfRule type="duplicateValues" dxfId="40" priority="56" stopIfTrue="1"/>

</xml_diff>